<commit_message>
Fix 5mm terminal in BOM
Same part was on two lines in BOM, combine / fix in source and regenerate.
</commit_message>
<xml_diff>
--- a/Source/Project Outputs for RUMBA_plus/RUMBA_plus_1_4_2A_BOM.xlsx
+++ b/Source/Project Outputs for RUMBA_plus/RUMBA_plus_1_4_2A_BOM.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BD384B1-8794-4C8F-B0DA-57D281524ACC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69699B33-CDB8-42D2-925A-EB59F2C058E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1035" windowWidth="4110" windowHeight="10725" xr2:uid="{ED978A29-247A-4233-81ED-B0EF55EC4E6A}"/>
+    <workbookView xWindow="1035" yWindow="1035" windowWidth="4110" windowHeight="10725" xr2:uid="{E70BCA24-BCAC-4C8A-8492-EE748680D711}"/>
   </bookViews>
   <sheets>
-    <sheet name="RUMBA_plus_BOM_1_4_2A" sheetId="1" r:id="rId1"/>
+    <sheet name="RUMBA_plus_1_4_2A_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="216">
   <si>
     <t>Designator</t>
   </si>
@@ -592,67 +592,61 @@
     <t>311-140KHRCT-ND</t>
   </si>
   <si>
-    <t>HB-PWR, MAIN-PWR</t>
-  </si>
-  <si>
-    <t>Screw Terminal 5mm 2-Way</t>
+    <t>E0_MS, E1_MS, E2_MS, X_MS, Y_MS, Z_MS</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE DIP SPST 25MA 24V</t>
+  </si>
+  <si>
+    <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t>416131160803</t>
+  </si>
+  <si>
+    <t>732-3853-1-ND</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>APEM</t>
+  </si>
+  <si>
+    <t>MJTP1106SATR</t>
+  </si>
+  <si>
+    <t>679-2396-1-ND</t>
+  </si>
+  <si>
+    <t>FAN0, FAN1, HE0, HE1, HE2</t>
+  </si>
+  <si>
+    <t>TERM BLK 2POS SIDE ENT 3.5MM PCB</t>
   </si>
   <si>
     <t>Phoenix Contact</t>
   </si>
   <si>
+    <t>MKDS1/2-3,5</t>
+  </si>
+  <si>
+    <t>277-5719-ND</t>
+  </si>
+  <si>
+    <t>HB-OUT, HB-PWR, MAIN-PWR</t>
+  </si>
+  <si>
+    <t>TERM BLK 2POS SIDE ENTRY 5MM PCB</t>
+  </si>
+  <si>
     <t>1935776</t>
   </si>
   <si>
     <t>277-6405-ND</t>
-  </si>
-  <si>
-    <t>E0_MS, E1_MS, E2_MS, X_MS, Y_MS, Z_MS</t>
-  </si>
-  <si>
-    <t>SWITCH SLIDE DIP SPST 25MA 24V</t>
-  </si>
-  <si>
-    <t>Wurth Electronics</t>
-  </si>
-  <si>
-    <t>416131160803</t>
-  </si>
-  <si>
-    <t>732-3853-1-ND</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
-  </si>
-  <si>
-    <t>APEM</t>
-  </si>
-  <si>
-    <t>MJTP1106SATR</t>
-  </si>
-  <si>
-    <t>679-2396-1-ND</t>
-  </si>
-  <si>
-    <t>FAN0, FAN1, HE0, HE1, HE2</t>
-  </si>
-  <si>
-    <t>TERM BLK 2POS SIDE ENT 3.5MM PCB</t>
-  </si>
-  <si>
-    <t>MKDS1/2-3,5</t>
-  </si>
-  <si>
-    <t>277-5719-ND</t>
-  </si>
-  <si>
-    <t>HB-OUT</t>
-  </si>
-  <si>
-    <t>TERM BLK 2POS SIDE ENTRY 5MM PCB</t>
   </si>
   <si>
     <t>E0_MOT, E1_MOT, E2_MOT, X_MOT, Y_MOT, Z_MOT</t>
@@ -1073,8 +1067,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E7E2C8-73B6-45E8-B6DD-185367C2FFCC}">
-  <dimension ref="A1:H50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A310E97-4643-4F2C-A7EF-E3FEC2F4018E}">
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1082,12 +1076,12 @@
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2216,7 +2210,7 @@
         <v>189</v>
       </c>
       <c r="C44" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>17</v>
@@ -2242,7 +2236,7 @@
         <v>194</v>
       </c>
       <c r="C45" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>17</v>
@@ -2268,7 +2262,7 @@
         <v>199</v>
       </c>
       <c r="C46" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
@@ -2294,13 +2288,13 @@
         <v>204</v>
       </c>
       <c r="C47" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>205</v>
@@ -2320,227 +2314,198 @@
         <v>208</v>
       </c>
       <c r="C48" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C49" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" tooltip="Component" display="'Sullins" xr:uid="{18FFE07C-B9D6-4B6A-9734-A9069DC905FB}"/>
-    <hyperlink ref="F2" r:id="rId2" tooltip="Manufacturer" display="'QPC02SXGN-RC" xr:uid="{EE0B2014-7C08-4DC1-AAF3-EBC5F47E7E94}"/>
-    <hyperlink ref="H2" r:id="rId3" tooltip="Supplier" display="'S9337-ND" xr:uid="{7B98D141-3763-4804-9692-9B108BEC5204}"/>
-    <hyperlink ref="E3" r:id="rId4" tooltip="Component" display="'Panasonic" xr:uid="{0AE861E4-17DA-449F-BDDC-0F25F7EEBF5A}"/>
-    <hyperlink ref="F3" r:id="rId5" tooltip="Manufacturer" display="'EEEFT1V101AP" xr:uid="{A7D344B5-74FB-47C7-A563-2D8350F7A90B}"/>
-    <hyperlink ref="H3" r:id="rId6" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{7FB3CC7E-FB9C-4241-9866-E7E0F2AC6C6E}"/>
-    <hyperlink ref="E4" r:id="rId7" tooltip="Component" display="'Yageo" xr:uid="{B3C8EE4F-DE55-48BC-8CC3-FE0439D9AFB9}"/>
-    <hyperlink ref="F4" r:id="rId8" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{5D795B99-B5AD-482C-A5B9-FE03A6E0E22D}"/>
-    <hyperlink ref="H4" r:id="rId9" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{83CC2747-B1A8-4655-B140-12A4C843044C}"/>
-    <hyperlink ref="E5" r:id="rId10" tooltip="Component" display="'Taiyo Yuden" xr:uid="{8DDE42DC-F9B8-43B0-A536-5370D6E26F24}"/>
-    <hyperlink ref="F5" r:id="rId11" tooltip="Manufacturer" display="'EMK107B7105KA-T" xr:uid="{EB4329E6-37EF-4D80-94A0-08E4C8036849}"/>
-    <hyperlink ref="H5" r:id="rId12" tooltip="Supplier" display="'587-1241-1-ND" xr:uid="{A230B8EE-B33D-4EEE-9FD6-91BEF1195130}"/>
-    <hyperlink ref="E6" r:id="rId13" tooltip="Component" display="'TDK" xr:uid="{4AE40066-9B9C-49F5-801E-7C72D31EC668}"/>
-    <hyperlink ref="F6" r:id="rId14" tooltip="Manufacturer" display="'C2012X7R1A475K085AC" xr:uid="{AE2A619B-4CD7-4FE5-BD4A-535B6525EB3F}"/>
-    <hyperlink ref="H6" r:id="rId15" tooltip="Supplier" display="'445-14527-1-ND" xr:uid="{E8DD9280-DF20-4A73-BB21-60708746463B}"/>
-    <hyperlink ref="E7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{C0E39A4B-9BE8-46C6-A072-116D86C2AC71}"/>
-    <hyperlink ref="F7" r:id="rId17" tooltip="Manufacturer" display="'C1210C475K5RACTU" xr:uid="{E91002BD-CD2E-441F-84F2-63EE7C3DCB2B}"/>
-    <hyperlink ref="H7" r:id="rId18" tooltip="Supplier" display="'399-6785-1-ND" xr:uid="{BF7EA0E6-8C12-49CC-BFB1-FA1706DFF7E6}"/>
-    <hyperlink ref="E8" r:id="rId19" tooltip="Component" display="'Kyocera AVX" xr:uid="{F3229103-2999-4BC2-BC46-43B47C87488D}"/>
-    <hyperlink ref="F8" r:id="rId20" tooltip="Manufacturer" display="'06035C220JAT2A" xr:uid="{8E1D1029-5D55-4291-A342-1A273345895F}"/>
-    <hyperlink ref="H8" r:id="rId21" tooltip="Supplier" display="'478-6204-1-ND" xr:uid="{68F635F1-43C4-42D3-ADE5-1112F06C3EEB}"/>
-    <hyperlink ref="E9" r:id="rId22" tooltip="Component" display="'Molex" xr:uid="{D4EEA83F-2E5B-4C84-9453-4260B9D1A37A}"/>
-    <hyperlink ref="F9" r:id="rId23" tooltip="Manufacturer" display="'105017-0001" xr:uid="{A87ACEDF-4AC8-4F84-927D-51C7593EDF35}"/>
-    <hyperlink ref="H9" r:id="rId24" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{03EFD7C6-11BD-47A5-A136-C42566C4D48F}"/>
-    <hyperlink ref="E10" r:id="rId25" tooltip="Component" display="'Epson" xr:uid="{CF188930-39CA-4FE7-ABF4-79BE5D351389}"/>
-    <hyperlink ref="F10" r:id="rId26" tooltip="Manufacturer" display="'FA-23816.0000MBC3" xr:uid="{600102B5-8561-4673-9F0E-DF27E9DB6C96}"/>
-    <hyperlink ref="H10" r:id="rId27" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{D0B776FB-153F-4C25-AAB1-C7AD189BDC8C}"/>
-    <hyperlink ref="E11" r:id="rId28" tooltip="Component" display="'MCC" xr:uid="{CF07150C-7C2C-4293-BB6D-7C600D9F2F8C}"/>
-    <hyperlink ref="F11" r:id="rId29" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{EA387FDA-61FC-4E5D-9EAC-5EF07BF49F18}"/>
-    <hyperlink ref="H11" r:id="rId30" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{CC8131CC-B24D-4D6A-BFDC-C9DEE81047BA}"/>
-    <hyperlink ref="E12" r:id="rId31" tooltip="Component" display="'Diodes" xr:uid="{51E6A4A0-41B1-4E59-B697-F97EE92B663D}"/>
-    <hyperlink ref="F12" r:id="rId32" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{E5D1EDD0-9DA5-43E4-A281-61DC2DA09215}"/>
-    <hyperlink ref="H12" r:id="rId33" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{A509BDC4-4399-4AC3-A311-48D027D2FDC6}"/>
-    <hyperlink ref="E13" r:id="rId34" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{1132AEFC-EC2E-4A94-8B4F-75B20695EA41}"/>
-    <hyperlink ref="F13" r:id="rId35" tooltip="Manufacturer" display="'SS24FL" xr:uid="{A436CABE-5064-43A0-AB87-688B0B881FBC}"/>
-    <hyperlink ref="H13" r:id="rId36" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{36964338-A09C-44BA-B63B-CA6C1F13614E}"/>
-    <hyperlink ref="E14" r:id="rId37" tooltip="Component" display="'General Instruments" xr:uid="{03EB735C-A646-488D-A1E1-A2CEE9616D5A}"/>
-    <hyperlink ref="F14" r:id="rId38" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{C28C8AB6-9553-4F55-9C68-95D60C467C58}"/>
-    <hyperlink ref="H14" r:id="rId39" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{46A32CB5-DAEB-4CB6-AD51-5F193A249DBB}"/>
-    <hyperlink ref="E15" r:id="rId40" tooltip="Component" display="'Murata" xr:uid="{39AB10D9-5921-4DC9-A812-F5604178B0C4}"/>
-    <hyperlink ref="F15" r:id="rId41" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{58D602EC-9DD9-468A-AFB4-A0AA486DA142}"/>
-    <hyperlink ref="H15" r:id="rId42" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{62E8DF54-324F-431A-9DF8-AA9CC10B6CA3}"/>
-    <hyperlink ref="E16" r:id="rId43" tooltip="Component" display="'Bourns" xr:uid="{973710B0-073E-43E6-9110-A1A8125A9CB6}"/>
-    <hyperlink ref="F16" r:id="rId44" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{AC2EBE50-B138-4E87-B5D9-8799E67612F1}"/>
-    <hyperlink ref="H16" r:id="rId45" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{558932F0-8975-4F28-9C42-40A3E4D39E22}"/>
-    <hyperlink ref="E17" r:id="rId46" tooltip="Component" display="'Bourns" xr:uid="{73563059-8E9E-4215-A45B-A2CBF1097B1D}"/>
-    <hyperlink ref="F17" r:id="rId47" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{467E5FA0-DEA9-4A3D-9B24-13565C1598B0}"/>
-    <hyperlink ref="H17" r:id="rId48" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{CB22681E-7653-4820-9553-3CAF97895E23}"/>
-    <hyperlink ref="E18" r:id="rId49" tooltip="Component" display="'Memory Protection Devices" xr:uid="{CF94C808-FAC5-4D1F-8E50-EDD5BC35F8A5}"/>
-    <hyperlink ref="F18" r:id="rId50" tooltip="Manufacturer" display="'BK-6013" xr:uid="{25387055-DB07-4B11-A2AD-AFE393873C7E}"/>
-    <hyperlink ref="H18" r:id="rId51" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{26AC93FE-B107-4927-97C1-DD54E3D648B7}"/>
-    <hyperlink ref="E19" tooltip="Component" display="'Generic Header" xr:uid="{17981523-1AAB-41E4-8FFF-E371BCD3B8C0}"/>
-    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{DF814CA7-B673-4654-8D91-29971A0DDBEA}"/>
-    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{A0B866E5-89D8-48CC-A44D-4C63F4FEB815}"/>
-    <hyperlink ref="E20" tooltip="Component" display="'Generic Header" xr:uid="{0147D1A4-BC0D-48DA-A186-C8A9D0179765}"/>
-    <hyperlink ref="F20" tooltip="Manufacturer" display="'" xr:uid="{9617B630-C11C-47ED-A821-A488CAF1D6EE}"/>
-    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{686298E3-C983-4033-A2C5-9B0DC0383B2F}"/>
-    <hyperlink ref="E21" tooltip="Component" display="'Generic Header" xr:uid="{74E654E8-CCBE-409B-8785-A668B173CBB6}"/>
-    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{8E86070A-8272-4628-AFC1-463F125554A7}"/>
-    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{D625EA45-8CA4-468D-8BDA-4F556B2BB602}"/>
-    <hyperlink ref="E22" tooltip="Component" display="'Generic Header" xr:uid="{651F0FF8-BF33-4BC6-A987-C97D90248F13}"/>
-    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{0552AE54-19FE-40EB-9E6F-78F2E554CE60}"/>
-    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{73BD28F3-56CF-4BC7-A9BB-8A29DB387BC7}"/>
-    <hyperlink ref="E23" tooltip="Component" display="'Generic Header" xr:uid="{B3FDF792-9259-4982-8069-0A842B39EABA}"/>
-    <hyperlink ref="F23" tooltip="Manufacturer" display="'" xr:uid="{76A80EDB-7768-40FC-867E-7C3609EE4B5D}"/>
-    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{CD2059CF-9D99-457C-BAF1-C05ACACFA4DC}"/>
-    <hyperlink ref="E24" tooltip="Component" display="'Generic Header" xr:uid="{437DA3E8-DCFD-4D43-BC38-D612278C4B6C}"/>
-    <hyperlink ref="F24" tooltip="Manufacturer" display="'" xr:uid="{BDF11DF0-270F-4774-B723-69B5D32D4A11}"/>
-    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{28B3DF9F-F730-445A-8DAE-48940E867683}"/>
-    <hyperlink ref="E25" tooltip="Component" display="'Generic Header" xr:uid="{65C6AC99-5CF8-4408-9B76-BDB5BC8B9556}"/>
-    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{C7370E5A-7EE5-4C75-B3B1-5FD4343FDA92}"/>
-    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{8B8E38EA-5711-4AC7-B325-6F190DF2AEB8}"/>
-    <hyperlink ref="E26" tooltip="Component" display="'Generic Header" xr:uid="{8C0E7341-A0F3-4FA7-89F9-46DC5AC28178}"/>
-    <hyperlink ref="F26" tooltip="Manufacturer" display="'" xr:uid="{47CED069-12FD-457D-9EE7-55BCB610C355}"/>
-    <hyperlink ref="H26" tooltip="Supplier" display="'" xr:uid="{29853A20-91F7-4608-8659-8B51823DADAB}"/>
-    <hyperlink ref="E27" r:id="rId52" tooltip="Component" display="'Microchip" xr:uid="{D0CA0E5C-C7C4-41A2-8939-8C6E6972A3D4}"/>
-    <hyperlink ref="F27" r:id="rId53" tooltip="Manufacturer" display="'ATMEGA16U2-MU" xr:uid="{7B4DE4F3-6BCE-4A19-BF7B-EE9621FC6A06}"/>
-    <hyperlink ref="H27" r:id="rId54" tooltip="Supplier" display="'ATMEGA16U2-MU-ND" xr:uid="{658E5DF8-79DC-4BC8-90D2-61F9982FBF29}"/>
-    <hyperlink ref="E28" r:id="rId55" tooltip="Component" display="'Microchip / Atmel" xr:uid="{8832A901-2E87-4825-9159-9BFB4D42D0B3}"/>
-    <hyperlink ref="F28" r:id="rId56" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{198EE85A-7696-45F2-82D8-832AA4C096F8}"/>
-    <hyperlink ref="H28" r:id="rId57" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{51CA8A4E-C153-4DD3-AD06-09615A52FA58}"/>
-    <hyperlink ref="E29" r:id="rId58" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{9386B762-A9E8-45F6-9DF5-29E51663B8F8}"/>
-    <hyperlink ref="F29" r:id="rId59" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{ACA6B6E8-C00D-4019-992D-A7D09409D165}"/>
-    <hyperlink ref="H29" r:id="rId60" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{E4FB99C1-90D1-491E-9090-69A3FD479155}"/>
-    <hyperlink ref="E30" r:id="rId61" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{6C8C9BFB-E9D4-40B3-850C-3B1828B8BC44}"/>
-    <hyperlink ref="F30" r:id="rId62" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{7DF4A19A-7745-45D3-8141-E0D11AD7564E}"/>
-    <hyperlink ref="H30" r:id="rId63" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{1CCA2ABF-6CBD-449C-814F-9646BB01B852}"/>
-    <hyperlink ref="E31" r:id="rId64" tooltip="Component" display="'Vishay Lite-On" xr:uid="{6AA8530B-B4C6-4151-925F-4A2E8D07DB82}"/>
-    <hyperlink ref="F31" r:id="rId65" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{ED9556D0-7F9F-4002-B53D-C14E08EB6B4D}"/>
-    <hyperlink ref="H31" r:id="rId66" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{1E34BE3D-5018-4DB3-B177-8D0AA8ABFFEB}"/>
-    <hyperlink ref="E32" r:id="rId67" tooltip="Component" display="'Vishay Lite-On" xr:uid="{3F92821E-E531-42A9-8E2F-996E7C67D9FE}"/>
-    <hyperlink ref="F32" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{44AC24A8-C3C2-4284-948F-3ACE65253177}"/>
-    <hyperlink ref="H32" r:id="rId69" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{1F39453E-CAF5-4E22-8115-E5588A6D1E9F}"/>
-    <hyperlink ref="E33" r:id="rId70" tooltip="Component" display="'Nexperia" xr:uid="{CD214499-CCF8-454D-B1C8-180D0E9BFBD1}"/>
-    <hyperlink ref="F33" r:id="rId71" tooltip="Manufacturer" display="'BUK9Y21-40E,115" xr:uid="{A6EAEBA3-20E7-4CAD-A674-3B21FBDB7D77}"/>
-    <hyperlink ref="H33" r:id="rId72" tooltip="Supplier" display="'1727-1123-1-ND" xr:uid="{541E6359-FE0D-4082-9A91-CF792109EA4E}"/>
-    <hyperlink ref="E34" r:id="rId73" tooltip="Component" display="'Nexperia" xr:uid="{FCAA6503-7162-4D04-A7DB-B9DA6FCC4712}"/>
-    <hyperlink ref="F34" r:id="rId74" tooltip="Manufacturer" display="'PSMN1R8-40YLC,115" xr:uid="{53C7FE7D-7D10-4BE7-B068-E2B73F494C45}"/>
-    <hyperlink ref="H34" r:id="rId75" tooltip="Supplier" display="'1727-1052-1-ND" xr:uid="{7781CD66-3E96-432F-8E17-06F38D98380B}"/>
-    <hyperlink ref="E35" r:id="rId76" tooltip="Component" display="'Bel" xr:uid="{A529F792-C65B-4CEC-B3AE-21958BBFA38C}"/>
-    <hyperlink ref="F35" r:id="rId77" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{A015EF64-DBC5-47F1-A887-430C7DE765F1}"/>
-    <hyperlink ref="H35" r:id="rId78" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{8F15F700-2C53-42C8-96C8-D9900EF9FA0B}"/>
-    <hyperlink ref="E36" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{DBE8B3BC-D024-47EC-9B26-28C5B489E79C}"/>
-    <hyperlink ref="F36" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{5B657405-52CB-472C-A3B1-500B622EF0AF}"/>
-    <hyperlink ref="H36" r:id="rId81" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{B51AA361-47C4-4467-957B-7ED0506042A1}"/>
-    <hyperlink ref="E37" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{42C95FA4-3040-495D-9E40-D1BF593E2C19}"/>
-    <hyperlink ref="F37" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{A3D9121D-8D97-40DF-845F-280229F492A8}"/>
-    <hyperlink ref="H37" r:id="rId84" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{DEB0C63B-8D40-473E-A5C1-5B9E04E92E41}"/>
-    <hyperlink ref="E38" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{A8CCBA26-7C17-45E8-B9FF-E6DC24226774}"/>
-    <hyperlink ref="F38" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{7A04B63B-C092-4063-A382-F46A49DC1EC0}"/>
-    <hyperlink ref="H38" r:id="rId87" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{ED3B3D1B-05B2-42E5-B405-E678AF5D1F89}"/>
-    <hyperlink ref="E39" r:id="rId88" tooltip="Component" display="'Yageo Phycomp" xr:uid="{C170B6C2-C908-4D18-B882-805BF091394A}"/>
-    <hyperlink ref="F39" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{77B54149-1DD0-4A2A-9EC3-179464E0D1A5}"/>
-    <hyperlink ref="H39" r:id="rId90" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{42A39318-97FF-43D5-8DE2-6D6EBAFA1030}"/>
-    <hyperlink ref="E40" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{4BC6B98F-2A2C-4187-9401-A927410A92B0}"/>
-    <hyperlink ref="F40" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{7A8C26E9-8B69-4E0A-B726-310C63310E45}"/>
-    <hyperlink ref="H40" r:id="rId93" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{7142CFE1-C29D-490C-AB33-D6A1EA7DAC23}"/>
-    <hyperlink ref="E41" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{1C8EE593-F1D5-4DBC-893B-6FE18DE55873}"/>
-    <hyperlink ref="F41" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{A9563202-E7A3-4487-9BDD-7EDA0FC00F62}"/>
-    <hyperlink ref="H41" r:id="rId96" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{5885893E-A5A7-4A91-9627-EEEDBD6AB421}"/>
-    <hyperlink ref="E42" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{BCD7CE7F-E90B-46C5-8A50-26CBC581EA92}"/>
-    <hyperlink ref="F42" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{042C247A-8F67-45E8-8FD4-7B34B26C5BD4}"/>
-    <hyperlink ref="H42" r:id="rId99" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{60A590F5-56E5-46BB-8E4C-9685D7D9F731}"/>
-    <hyperlink ref="E43" r:id="rId100" tooltip="Component" display="'Yageo" xr:uid="{82B6DFAC-D5E9-4791-B4B3-60E3600097B2}"/>
-    <hyperlink ref="F43" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{66B160E5-8231-4954-94B0-4100EA04B270}"/>
-    <hyperlink ref="H43" r:id="rId102" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{2E56ADC8-FB9B-44AE-AFFD-B5E96D2A3D78}"/>
-    <hyperlink ref="E44" r:id="rId103" tooltip="Component" display="'Phoenix Contact" xr:uid="{088E67CA-220E-4BD5-9E76-733A3E8D23A9}"/>
-    <hyperlink ref="F44" r:id="rId104" tooltip="Manufacturer" display="'1935776" xr:uid="{F695651C-14DB-4EA2-9F09-2E6E93D61B80}"/>
-    <hyperlink ref="H44" r:id="rId105" tooltip="Supplier" display="'277-6405-ND" xr:uid="{B04DC7E3-F4A7-4920-BFC7-17D36F1EB94A}"/>
-    <hyperlink ref="E45" r:id="rId106" tooltip="Component" display="'Wurth Electronics" xr:uid="{CC6DA31F-7290-4B80-9764-BC58FB1B7DCA}"/>
-    <hyperlink ref="F45" r:id="rId107" tooltip="Manufacturer" display="'416131160803" xr:uid="{FFD27985-E647-4168-B2D0-0B70A5F79680}"/>
-    <hyperlink ref="H45" r:id="rId108" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{5DF1E3B3-E753-4C3F-A835-0E640EAE7807}"/>
-    <hyperlink ref="E46" r:id="rId109" tooltip="Component" display="'APEM" xr:uid="{22FEE83A-2045-4BD7-B215-B781D11D260C}"/>
-    <hyperlink ref="F46" r:id="rId110" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{EADA80B8-FA87-41DC-BB69-E959AA5B0501}"/>
-    <hyperlink ref="H46" r:id="rId111" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{98E18E9B-C028-4653-B781-5AA5C3F68B66}"/>
-    <hyperlink ref="E47" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{F50F065E-564B-4064-9EB5-B3DBBC62BE0C}"/>
-    <hyperlink ref="F47" r:id="rId113" tooltip="Manufacturer" display="'MKDS1/2-3,5" xr:uid="{A0143C42-7365-45FB-818D-2343B688B629}"/>
-    <hyperlink ref="H47" r:id="rId114" tooltip="Supplier" display="'277-5719-ND" xr:uid="{8DF0C021-49C5-4E3C-8E46-2955015D4F8C}"/>
-    <hyperlink ref="E48" r:id="rId115" tooltip="Component" display="'Phoenix Contact" xr:uid="{ED4A4352-F6E8-4B05-9947-9A7EFEA54AFD}"/>
-    <hyperlink ref="F48" r:id="rId116" tooltip="Manufacturer" display="'1935776" xr:uid="{37235D55-5EB8-4FEB-9CB3-BC40A227B48F}"/>
-    <hyperlink ref="H48" r:id="rId117" tooltip="Supplier" display="'277-6405-ND" xr:uid="{E8C8FE7F-A5BD-4D3C-B307-62BC4AEBD150}"/>
-    <hyperlink ref="E49" r:id="rId118" tooltip="Component" display="'Phoenix Contact" xr:uid="{71C3241E-BCEF-4F45-BE8A-1956001D2C20}"/>
-    <hyperlink ref="F49" r:id="rId119" tooltip="Manufacturer" display="'MKDS1/4-3,5" xr:uid="{252646B8-4648-4A50-9839-CF73079B3A17}"/>
-    <hyperlink ref="H49" r:id="rId120" tooltip="Supplier" display="'277-5744-ND" xr:uid="{46A0B8D6-B076-4370-A067-801D7E59C8D9}"/>
-    <hyperlink ref="E50" r:id="rId121" tooltip="Component" display="'STMicroelectronics" xr:uid="{7E849632-75DA-4593-9591-8782F9AAA5E0}"/>
-    <hyperlink ref="F50" r:id="rId122" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{55F6D486-0982-41B4-A76F-387F13064C0A}"/>
-    <hyperlink ref="H50" r:id="rId123" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{8CD75313-3DFD-4D91-8BC3-D24DC503E9BC}"/>
+    <hyperlink ref="E2" r:id="rId1" tooltip="Component" display="'Sullins" xr:uid="{968D0E8C-E264-4757-8B5B-F8729179FAA8}"/>
+    <hyperlink ref="F2" r:id="rId2" tooltip="Manufacturer" display="'QPC02SXGN-RC" xr:uid="{3A259D1A-C8D6-4A68-AF0B-F9E84B5BF698}"/>
+    <hyperlink ref="H2" r:id="rId3" tooltip="Supplier" display="'S9337-ND" xr:uid="{5A55CBB3-E246-409D-87D7-9C28414BE66F}"/>
+    <hyperlink ref="E3" r:id="rId4" tooltip="Component" display="'Panasonic" xr:uid="{EB5AC404-4900-4A80-A2F6-30827D1FF4B9}"/>
+    <hyperlink ref="F3" r:id="rId5" tooltip="Manufacturer" display="'EEEFT1V101AP" xr:uid="{C27514B6-5A42-41A1-865D-0A9933033B02}"/>
+    <hyperlink ref="H3" r:id="rId6" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{8430A3B2-DB52-4C10-9072-5B1A7CB7F1BF}"/>
+    <hyperlink ref="E4" r:id="rId7" tooltip="Component" display="'Yageo" xr:uid="{69C69036-6429-4349-BF8F-E5A7212A5511}"/>
+    <hyperlink ref="F4" r:id="rId8" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{1298FC2D-C313-4A52-AD45-BEE14BBB19BB}"/>
+    <hyperlink ref="H4" r:id="rId9" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{333C80B1-69A8-4A02-8208-94AE7ACC6260}"/>
+    <hyperlink ref="E5" r:id="rId10" tooltip="Component" display="'Taiyo Yuden" xr:uid="{632E2916-E95E-4AA3-A8CD-1B5C9D5403FC}"/>
+    <hyperlink ref="F5" r:id="rId11" tooltip="Manufacturer" display="'EMK107B7105KA-T" xr:uid="{96EE8B45-599C-48BD-B1ED-C4208B5B2C9C}"/>
+    <hyperlink ref="H5" r:id="rId12" tooltip="Supplier" display="'587-1241-1-ND" xr:uid="{4C1FFDAD-BA0A-4B8C-B99A-3E053A9615EA}"/>
+    <hyperlink ref="E6" r:id="rId13" tooltip="Component" display="'TDK" xr:uid="{D9006911-2E9C-4E0A-A280-B43E3A04DD2D}"/>
+    <hyperlink ref="F6" r:id="rId14" tooltip="Manufacturer" display="'C2012X7R1A475K085AC" xr:uid="{054583CF-ED97-443D-924D-6D260563D04C}"/>
+    <hyperlink ref="H6" r:id="rId15" tooltip="Supplier" display="'445-14527-1-ND" xr:uid="{815A05C7-7215-4A04-A512-BEF88F8CB0BE}"/>
+    <hyperlink ref="E7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{EA44CAC7-443E-47B5-9CD0-F4A55C9D3D1D}"/>
+    <hyperlink ref="F7" r:id="rId17" tooltip="Manufacturer" display="'C1210C475K5RACTU" xr:uid="{7F8BC83B-F0A2-400B-80A4-3ED79574C53B}"/>
+    <hyperlink ref="H7" r:id="rId18" tooltip="Supplier" display="'399-6785-1-ND" xr:uid="{D8FD8B0F-A345-4FA8-A4EC-BABC05F08F96}"/>
+    <hyperlink ref="E8" r:id="rId19" tooltip="Component" display="'Kyocera AVX" xr:uid="{8D537837-0655-49CD-9FA0-E78413479153}"/>
+    <hyperlink ref="F8" r:id="rId20" tooltip="Manufacturer" display="'06035C220JAT2A" xr:uid="{2ECE4ECD-7EF1-4221-BD6F-24EE4D4CED7F}"/>
+    <hyperlink ref="H8" r:id="rId21" tooltip="Supplier" display="'478-6204-1-ND" xr:uid="{A918053C-735E-4A7D-BFCE-C4E28DA2C61F}"/>
+    <hyperlink ref="E9" r:id="rId22" tooltip="Component" display="'Molex" xr:uid="{0BB4D920-7876-457A-9717-54682FA1228F}"/>
+    <hyperlink ref="F9" r:id="rId23" tooltip="Manufacturer" display="'105017-0001" xr:uid="{0A394AC6-C695-41EA-B8EA-AC4644547172}"/>
+    <hyperlink ref="H9" r:id="rId24" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{D13FAB76-5308-43FA-975F-A95413FF43B5}"/>
+    <hyperlink ref="E10" r:id="rId25" tooltip="Component" display="'Epson" xr:uid="{1F107096-D020-4D57-BBFD-8617545B52E5}"/>
+    <hyperlink ref="F10" r:id="rId26" tooltip="Manufacturer" display="'FA-23816.0000MBC3" xr:uid="{31727DCC-3BE3-48CE-8FD4-2EFDB4A11E73}"/>
+    <hyperlink ref="H10" r:id="rId27" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{475AEC55-D8E5-43FB-BBE5-8FA9B872DADF}"/>
+    <hyperlink ref="E11" r:id="rId28" tooltip="Component" display="'MCC" xr:uid="{A3F5DABD-B806-48B9-BFFC-4A8BB3C54216}"/>
+    <hyperlink ref="F11" r:id="rId29" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{2114553A-8C8D-4B97-9E7D-66484D1AC910}"/>
+    <hyperlink ref="H11" r:id="rId30" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{9EFC2350-A0E2-4A58-9353-9946486DEFB8}"/>
+    <hyperlink ref="E12" r:id="rId31" tooltip="Component" display="'Diodes" xr:uid="{690407A6-6EA5-4F1D-A60F-00B8F4762F78}"/>
+    <hyperlink ref="F12" r:id="rId32" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{4D39F105-18A9-44B3-AE62-7E9C529522D0}"/>
+    <hyperlink ref="H12" r:id="rId33" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{FB2318FC-1CEA-4516-9823-342E78349355}"/>
+    <hyperlink ref="E13" r:id="rId34" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{4E4F84F2-5185-42F0-86FD-57FAAF97E7E9}"/>
+    <hyperlink ref="F13" r:id="rId35" tooltip="Manufacturer" display="'SS24FL" xr:uid="{CBEAA36F-5830-4D52-93C0-A4F4023FEE56}"/>
+    <hyperlink ref="H13" r:id="rId36" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{C46E322C-1B46-417B-8025-00909E55EC21}"/>
+    <hyperlink ref="E14" r:id="rId37" tooltip="Component" display="'General Instruments" xr:uid="{1D9E5376-87DA-4817-85B7-0742963064D7}"/>
+    <hyperlink ref="F14" r:id="rId38" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{5AF28CF8-5933-419B-A97E-3512FD6281DB}"/>
+    <hyperlink ref="H14" r:id="rId39" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{95D38656-6AA6-4DDC-B2B3-7BDFD2E8D595}"/>
+    <hyperlink ref="E15" r:id="rId40" tooltip="Component" display="'Murata" xr:uid="{C1ECC8BB-E507-4CF9-9701-6625FF1A3E11}"/>
+    <hyperlink ref="F15" r:id="rId41" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{90B91779-DFD9-4D05-B292-87A64EA558A9}"/>
+    <hyperlink ref="H15" r:id="rId42" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{6EEB8355-2529-4328-8E73-F9B2AC83A5DC}"/>
+    <hyperlink ref="E16" r:id="rId43" tooltip="Component" display="'Bourns" xr:uid="{9FD1DD88-6857-42CA-90E6-F766FDE4D2AE}"/>
+    <hyperlink ref="F16" r:id="rId44" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{BEF8AF03-CBCD-4C4A-98AE-BBE459A01DB8}"/>
+    <hyperlink ref="H16" r:id="rId45" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{54306C89-52F4-4D65-9CD7-6CB8B45E777B}"/>
+    <hyperlink ref="E17" r:id="rId46" tooltip="Component" display="'Bourns" xr:uid="{F1D17519-FF3E-4330-82EE-62EC46F3288E}"/>
+    <hyperlink ref="F17" r:id="rId47" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{9AA163F8-932E-4015-86F5-EC9038EC11CF}"/>
+    <hyperlink ref="H17" r:id="rId48" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{461EC537-6F35-435E-8400-80A041C28154}"/>
+    <hyperlink ref="E18" r:id="rId49" tooltip="Component" display="'Memory Protection Devices" xr:uid="{1B593CEE-DAF5-4688-AA27-C3937BBA52C1}"/>
+    <hyperlink ref="F18" r:id="rId50" tooltip="Manufacturer" display="'BK-6013" xr:uid="{60360EE8-7494-49C3-A559-51FD8158D85A}"/>
+    <hyperlink ref="H18" r:id="rId51" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{FD38A260-870C-4E3C-AEC5-FD3678D9B772}"/>
+    <hyperlink ref="E19" tooltip="Component" display="'Generic Header" xr:uid="{29336B69-1CD4-4E8E-A0BE-3C72933D2340}"/>
+    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{6DEA9FAE-5659-4EFF-A8D7-3C5166CC3BD1}"/>
+    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{ED4B894D-C366-4BCC-9330-F8218667A3ED}"/>
+    <hyperlink ref="E20" tooltip="Component" display="'Generic Header" xr:uid="{00B90512-B31D-4406-B8E0-964A4C5B338B}"/>
+    <hyperlink ref="F20" tooltip="Manufacturer" display="'" xr:uid="{F8DA7A3D-4DC1-43E8-BB51-0D5906E6C348}"/>
+    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{01F0A89F-5AAA-4D17-9507-18EDBBF3A9F3}"/>
+    <hyperlink ref="E21" tooltip="Component" display="'Generic Header" xr:uid="{5D1B5577-A906-4BC8-9526-C10D6E5BA67D}"/>
+    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{CA733CFC-BDB7-4E7A-94C6-44DF33A85A9E}"/>
+    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{145E4BBA-7D5A-43E3-9E80-B3205413A393}"/>
+    <hyperlink ref="E22" tooltip="Component" display="'Generic Header" xr:uid="{905E99FA-710A-4505-8E77-A2EF2A7929B0}"/>
+    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{70451FC8-6C2D-4812-8C13-4C0A93C84023}"/>
+    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{AAC3B58B-7D3F-499A-9F65-2F658455081C}"/>
+    <hyperlink ref="E23" tooltip="Component" display="'Generic Header" xr:uid="{F9EDDF67-8A2B-478C-B87C-2A7D07DC1B83}"/>
+    <hyperlink ref="F23" tooltip="Manufacturer" display="'" xr:uid="{BEC91BDC-BBFB-4ACC-95A0-BAFD3F5431EF}"/>
+    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{935056A1-CE1B-4BDE-B441-E7EEBD8BEBC9}"/>
+    <hyperlink ref="E24" tooltip="Component" display="'Generic Header" xr:uid="{75214B9D-5C8C-4B68-95B2-6AE2C59341C1}"/>
+    <hyperlink ref="F24" tooltip="Manufacturer" display="'" xr:uid="{46E6C33C-42FC-4AA0-B535-4301C002B270}"/>
+    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{D5528D46-88B5-408E-BE92-D43D3969F9CA}"/>
+    <hyperlink ref="E25" tooltip="Component" display="'Generic Header" xr:uid="{144B5E20-0049-486B-A2BD-DB0CA54BA8FB}"/>
+    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{5C532C4F-EF9E-4509-9658-CE22C27200E4}"/>
+    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{52D0C4F8-F307-4CB6-BC57-057435321817}"/>
+    <hyperlink ref="E26" tooltip="Component" display="'Generic Header" xr:uid="{3A884513-4FA0-4277-818B-89BED84FB8A5}"/>
+    <hyperlink ref="F26" tooltip="Manufacturer" display="'" xr:uid="{32CD951C-B778-4FDF-9F9C-4DAA3380CD83}"/>
+    <hyperlink ref="H26" tooltip="Supplier" display="'" xr:uid="{999E6854-65B1-41F3-8E9D-A64431F1E0C5}"/>
+    <hyperlink ref="E27" r:id="rId52" tooltip="Component" display="'Microchip" xr:uid="{3195AFA5-BF60-474E-9247-0A04960ECEB9}"/>
+    <hyperlink ref="F27" r:id="rId53" tooltip="Manufacturer" display="'ATMEGA16U2-MU" xr:uid="{4DECF356-C660-440B-81A6-0AE732444232}"/>
+    <hyperlink ref="H27" r:id="rId54" tooltip="Supplier" display="'ATMEGA16U2-MU-ND" xr:uid="{2E6C2AAB-E9FF-428D-9F88-5240F4A27355}"/>
+    <hyperlink ref="E28" r:id="rId55" tooltip="Component" display="'Microchip / Atmel" xr:uid="{9251B13A-FB49-4B24-85A1-2ADC4ED5C302}"/>
+    <hyperlink ref="F28" r:id="rId56" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{48BBAEBC-9AEF-44C6-8355-A6D27B429448}"/>
+    <hyperlink ref="H28" r:id="rId57" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{3A301433-A086-4086-AB1C-D6F09429CCA5}"/>
+    <hyperlink ref="E29" r:id="rId58" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{EF1C8527-9956-48DE-B8EA-4F93D2D0B467}"/>
+    <hyperlink ref="F29" r:id="rId59" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{2ABBC3F4-1036-40BA-A635-49E19839C750}"/>
+    <hyperlink ref="H29" r:id="rId60" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{0A9E099A-475C-4722-8378-F3CE1BB3531A}"/>
+    <hyperlink ref="E30" r:id="rId61" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{1BDFE91B-A8F4-408B-BFB1-3C3C4C6E0375}"/>
+    <hyperlink ref="F30" r:id="rId62" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{52B3D08F-EC52-427D-A6E7-E0288AD40927}"/>
+    <hyperlink ref="H30" r:id="rId63" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{782A92D1-1D1E-473D-B497-68999C367C60}"/>
+    <hyperlink ref="E31" r:id="rId64" tooltip="Component" display="'Vishay Lite-On" xr:uid="{731552BA-797D-4A2A-ADDF-DAA870F3C01F}"/>
+    <hyperlink ref="F31" r:id="rId65" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{D11BEF18-A6EF-4895-A93D-0AFB577E5F56}"/>
+    <hyperlink ref="H31" r:id="rId66" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{855D88D3-76B1-4276-BFBD-2F4E0F34210F}"/>
+    <hyperlink ref="E32" r:id="rId67" tooltip="Component" display="'Vishay Lite-On" xr:uid="{144EFC4E-4110-4556-A3F5-ECB8EEB85DAB}"/>
+    <hyperlink ref="F32" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{FFFA9BDB-3C43-4A5B-96F6-67130A1A0514}"/>
+    <hyperlink ref="H32" r:id="rId69" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{60BA805D-4A97-4DD4-93BF-A03B72F92DB9}"/>
+    <hyperlink ref="E33" r:id="rId70" tooltip="Component" display="'Nexperia" xr:uid="{5BB9ED0E-804F-4FE6-8E71-D4FC5C2F9106}"/>
+    <hyperlink ref="F33" r:id="rId71" tooltip="Manufacturer" display="'BUK9Y21-40E,115" xr:uid="{172D9B76-7170-4EEC-8C25-7D9C59410462}"/>
+    <hyperlink ref="H33" r:id="rId72" tooltip="Supplier" display="'1727-1123-1-ND" xr:uid="{B4915611-75D4-4549-BB8A-8FC6C254C1AD}"/>
+    <hyperlink ref="E34" r:id="rId73" tooltip="Component" display="'Nexperia" xr:uid="{D7874A4D-D663-42E2-95CD-246F12E14A21}"/>
+    <hyperlink ref="F34" r:id="rId74" tooltip="Manufacturer" display="'PSMN1R8-40YLC,115" xr:uid="{610AA18B-8B6C-4B70-B47E-A80FE0124201}"/>
+    <hyperlink ref="H34" r:id="rId75" tooltip="Supplier" display="'1727-1052-1-ND" xr:uid="{E47EAD35-97B1-452C-8C73-F912E11BF6C8}"/>
+    <hyperlink ref="E35" r:id="rId76" tooltip="Component" display="'Bel" xr:uid="{893B7A6B-056B-4E50-86FC-CD1743A729F7}"/>
+    <hyperlink ref="F35" r:id="rId77" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{F81CFA7F-8F7E-4C11-A6D7-A7877D343565}"/>
+    <hyperlink ref="H35" r:id="rId78" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{6FEAB7CD-EAE9-4923-99F5-C07A98E806D4}"/>
+    <hyperlink ref="E36" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{52CFA0DA-AF8D-4C6D-A5F8-4B9AC118123A}"/>
+    <hyperlink ref="F36" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{F7508EC3-2047-45BE-81C7-C9C0A49DFA07}"/>
+    <hyperlink ref="H36" r:id="rId81" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{C8D5BEDE-8466-4F7A-AE02-AB2DD0332593}"/>
+    <hyperlink ref="E37" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{C4EBE395-3476-42EB-9EBC-60DEB505145B}"/>
+    <hyperlink ref="F37" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{8697BB15-9216-40E4-996A-9EC03CE178DA}"/>
+    <hyperlink ref="H37" r:id="rId84" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{A6B015D8-9497-4742-B000-C0FC3B97DB8D}"/>
+    <hyperlink ref="E38" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{899C85BC-10C9-4C44-AA78-830E832678A3}"/>
+    <hyperlink ref="F38" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{15D37BA0-C1D2-41EF-B3B6-19C519B1383F}"/>
+    <hyperlink ref="H38" r:id="rId87" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{0BF9F661-B9DE-42CD-B3B9-845E287B71EC}"/>
+    <hyperlink ref="E39" r:id="rId88" tooltip="Component" display="'Yageo Phycomp" xr:uid="{06EEF875-9E1E-418B-B720-EE26A5870E4B}"/>
+    <hyperlink ref="F39" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{831667F8-F910-4175-BCC2-6869B07B3CD5}"/>
+    <hyperlink ref="H39" r:id="rId90" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{9478D5F6-84E9-4412-BE3D-5194463FE0DD}"/>
+    <hyperlink ref="E40" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{E7B060BA-597B-4ED8-8595-23124A463F88}"/>
+    <hyperlink ref="F40" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{3C02D33D-D6D5-4FA8-BC3D-2FFF05278355}"/>
+    <hyperlink ref="H40" r:id="rId93" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{14069EB5-8B29-4C8A-82DC-26145ABB3363}"/>
+    <hyperlink ref="E41" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{60143F7D-8080-4765-843C-BFD3B5FEF581}"/>
+    <hyperlink ref="F41" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{F2ED1F02-EBDA-40B1-8337-92D7542B94AE}"/>
+    <hyperlink ref="H41" r:id="rId96" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{3676D8C4-E489-4601-BD98-63AF90227B19}"/>
+    <hyperlink ref="E42" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{4072A16D-8B62-4705-A9AA-DDA7FD8E6F98}"/>
+    <hyperlink ref="F42" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{3BC8DF01-5911-466A-A1C3-E4A64245B266}"/>
+    <hyperlink ref="H42" r:id="rId99" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{32A21A1F-C00A-4366-B2F5-9051560263EE}"/>
+    <hyperlink ref="E43" r:id="rId100" tooltip="Component" display="'Yageo" xr:uid="{C94E959A-EC2B-4165-800C-2A19C2E3B4D3}"/>
+    <hyperlink ref="F43" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{A21527CE-6578-4CC0-9652-BBFD95A3F052}"/>
+    <hyperlink ref="H43" r:id="rId102" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{77240F23-9D50-4B6C-9D6B-F36414A9A2B6}"/>
+    <hyperlink ref="E44" r:id="rId103" tooltip="Component" display="'Wurth Electronics" xr:uid="{50C81BEA-33A3-42AE-A1BE-2A145BD6DB88}"/>
+    <hyperlink ref="F44" r:id="rId104" tooltip="Manufacturer" display="'416131160803" xr:uid="{DF58EE5F-E402-4445-BF08-AEE160161C56}"/>
+    <hyperlink ref="H44" r:id="rId105" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{393EC610-B2F1-4BF8-84E1-B089717B95BA}"/>
+    <hyperlink ref="E45" r:id="rId106" tooltip="Component" display="'APEM" xr:uid="{332FDA72-75C8-4E67-A6FC-E965354EEFA4}"/>
+    <hyperlink ref="F45" r:id="rId107" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{A8D580BF-0966-42A4-908B-B104724BA267}"/>
+    <hyperlink ref="H45" r:id="rId108" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{DC5284EC-944D-4965-9597-B793DD971B63}"/>
+    <hyperlink ref="E46" r:id="rId109" tooltip="Component" display="'Phoenix Contact" xr:uid="{D96B4B63-4B17-438E-ABF9-A5D310D8AD1B}"/>
+    <hyperlink ref="F46" r:id="rId110" tooltip="Manufacturer" display="'MKDS1/2-3,5" xr:uid="{8D256E76-4545-480F-A24A-1F0421756DEF}"/>
+    <hyperlink ref="H46" r:id="rId111" tooltip="Supplier" display="'277-5719-ND" xr:uid="{BBCE262C-DF8C-4C38-A0E9-C8A5B3CE7E74}"/>
+    <hyperlink ref="E47" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{C2F0362B-9B05-4A1A-9F50-FF6071721A39}"/>
+    <hyperlink ref="F47" r:id="rId113" tooltip="Manufacturer" display="'1935776" xr:uid="{CE0C2560-5A42-405A-AC1D-21C03E147C60}"/>
+    <hyperlink ref="H47" r:id="rId114" tooltip="Supplier" display="'277-6405-ND" xr:uid="{32127689-5B92-43B3-9111-45BCB41E9EBD}"/>
+    <hyperlink ref="E48" r:id="rId115" tooltip="Component" display="'Phoenix Contact" xr:uid="{77922A95-0152-4759-9934-B4740485314B}"/>
+    <hyperlink ref="F48" r:id="rId116" tooltip="Manufacturer" display="'MKDS1/4-3,5" xr:uid="{B75E61A6-F0F9-4F3C-B94E-B34FC649A5F3}"/>
+    <hyperlink ref="H48" r:id="rId117" tooltip="Supplier" display="'277-5744-ND" xr:uid="{AAD59821-C808-4EB8-BC90-DC9992EE939E}"/>
+    <hyperlink ref="E49" r:id="rId118" tooltip="Component" display="'STMicroelectronics" xr:uid="{EF65047E-7CC6-4485-A9C4-5327B0C3D4F8}"/>
+    <hyperlink ref="F49" r:id="rId119" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{2BF9253A-F67F-409F-B793-EA7D1E862D03}"/>
+    <hyperlink ref="H49" r:id="rId120" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{FC5E01C6-24FA-4BD0-B60D-5D3AF2F5493E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId124"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId121"/>
 </worksheet>
 </file>
</xml_diff>